<commit_message>
FInition de la helppage
</commit_message>
<xml_diff>
--- a/Documentation/Journaux/Evann-JournalDeTravail.xlsx
+++ b/Documentation/Journaux/Evann-JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
   <si>
     <t>Date de début</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Réussir a écrire le message que l'utilisateur envoie dans la base de donnée sur la page help</t>
+  </si>
+  <si>
+    <t>15h40</t>
+  </si>
+  <si>
+    <t>Continuer à coder la help page</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,13 +1081,25 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="3">
+        <v>45091</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45091</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>

</xml_diff>